<commit_message>
Added gamma_n function for V20
</commit_message>
<xml_diff>
--- a/plot4_timeseries_EN4/EN4_water_mass_limits_each_region.xlsx
+++ b/plot4_timeseries_EN4/EN4_water_mass_limits_each_region.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work_computer_sync\OSNAP_postdoc\iAtlantic\iAtlantic_region_trends\plot4_timeseries_EN4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCDE3AED-D8BB-438F-990E-020CC53AD77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48B69D5A-E475-4BA3-88C1-F45F56DA250E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="2610" windowWidth="16185" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
         <v>27.85</v>
       </c>
       <c r="D4" s="7">
-        <v>27.975000000000001</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,10 +581,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="7">
-        <v>27.975000000000001</v>
+        <v>27.95</v>
       </c>
       <c r="D5" s="7">
-        <v>28.05</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="8">
-        <v>28.05</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>10</v>
@@ -637,10 +637,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="7">
-        <v>27.9</v>
+        <v>27.85</v>
       </c>
       <c r="D9" s="7">
-        <v>28</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="8">
-        <v>28.05</v>
+        <v>28</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>10</v>
@@ -668,7 +668,7 @@
         <v>26.5</v>
       </c>
       <c r="D11" s="7">
-        <v>27.2</v>
+        <v>27.1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>27.5</v>
       </c>
       <c r="D12" s="7">
-        <v>27.8</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -693,10 +693,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="7">
+        <v>27.85</v>
+      </c>
+      <c r="D13" s="7">
         <v>27.9</v>
-      </c>
-      <c r="D13" s="7">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -707,10 +707,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="7">
-        <v>28</v>
+        <v>27.9</v>
       </c>
       <c r="D14" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>10</v>
@@ -763,10 +763,10 @@
         <v>13</v>
       </c>
       <c r="C18" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="D18" s="7">
         <v>27.9</v>
-      </c>
-      <c r="D18" s="7">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,10 +777,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="7">
-        <v>28</v>
+        <v>27.9</v>
       </c>
       <c r="D19" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>10</v>
@@ -836,7 +836,7 @@
         <v>26.8</v>
       </c>
       <c r="D23" s="7">
-        <v>27.3</v>
+        <v>27.1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,10 +847,10 @@
         <v>18</v>
       </c>
       <c r="C24" s="7">
-        <v>27.5</v>
+        <v>27.45</v>
       </c>
       <c r="D24" s="7">
-        <v>27.7</v>
+        <v>27.65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,10 +861,10 @@
         <v>13</v>
       </c>
       <c r="C25" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="D25" s="7">
         <v>27.9</v>
-      </c>
-      <c r="D25" s="7">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,10 +875,10 @@
         <v>14</v>
       </c>
       <c r="C26" s="7">
-        <v>28</v>
+        <v>27.9</v>
       </c>
       <c r="D26" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>10</v>
@@ -934,7 +934,7 @@
         <v>26.3</v>
       </c>
       <c r="D30" s="7">
-        <v>26.6</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,10 +945,10 @@
         <v>6</v>
       </c>
       <c r="C31" s="7">
-        <v>26.6</v>
+        <v>26.7</v>
       </c>
       <c r="D31" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>27.4</v>
       </c>
       <c r="D32" s="7">
-        <v>27.7</v>
+        <v>27.65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>13</v>
       </c>
       <c r="C33" s="7">
-        <v>27.75</v>
+        <v>27.7</v>
       </c>
       <c r="D33" s="7">
-        <v>27.9</v>
+        <v>27.85</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="7">
-        <v>27.9</v>
+        <v>27.85</v>
       </c>
       <c r="D34" s="7">
         <v>28</v>
@@ -1001,7 +1001,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>10</v>
@@ -1060,7 +1060,7 @@
         <v>26.6</v>
       </c>
       <c r="D39" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,7 +1074,7 @@
         <v>27.25</v>
       </c>
       <c r="D40" s="7">
-        <v>27.65</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1085,10 +1085,10 @@
         <v>13</v>
       </c>
       <c r="C41" s="7">
-        <v>27.8</v>
+        <v>27.75</v>
       </c>
       <c r="D41" s="7">
-        <v>27.95</v>
+        <v>27.9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,10 +1099,10 @@
         <v>14</v>
       </c>
       <c r="C42" s="7">
-        <v>27.95</v>
+        <v>27.9</v>
       </c>
       <c r="D42" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>22</v>
       </c>
       <c r="C43" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>10</v>
@@ -1158,7 +1158,7 @@
         <v>26.6</v>
       </c>
       <c r="D46" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,10 +1169,10 @@
         <v>18</v>
       </c>
       <c r="C47" s="7">
-        <v>27.25</v>
+        <v>27.3</v>
       </c>
       <c r="D47" s="7">
-        <v>27.65</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,10 +1183,10 @@
         <v>13</v>
       </c>
       <c r="C48" s="7">
-        <v>27.85</v>
+        <v>27.8</v>
       </c>
       <c r="D48" s="7">
-        <v>27.95</v>
+        <v>27.9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
         <v>14</v>
       </c>
       <c r="C49" s="7">
-        <v>27.95</v>
+        <v>27.9</v>
       </c>
       <c r="D49" s="7">
-        <v>28.05</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1211,7 @@
         <v>22</v>
       </c>
       <c r="C50" s="8">
-        <v>28.05</v>
+        <v>28</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>10</v>
@@ -1242,7 +1242,7 @@
         <v>26.6</v>
       </c>
       <c r="D52" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
         <v>27.25</v>
       </c>
       <c r="D53" s="7">
-        <v>27.65</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,10 +1267,10 @@
         <v>13</v>
       </c>
       <c r="C54" s="7">
-        <v>27.9</v>
+        <v>27.85</v>
       </c>
       <c r="D54" s="7">
-        <v>28</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>14</v>
       </c>
       <c r="C55" s="7">
-        <v>28</v>
+        <v>27.95</v>
       </c>
       <c r="D55" s="7">
-        <v>28.1</v>
+        <v>28.05</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
         <v>22</v>
       </c>
       <c r="C56" s="8">
-        <v>28.1</v>
+        <v>28.05</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>10</v>
@@ -1340,7 +1340,7 @@
         <v>26.6</v>
       </c>
       <c r="D59" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1351,10 +1351,10 @@
         <v>18</v>
       </c>
       <c r="C60" s="7">
-        <v>27.25</v>
+        <v>27.2</v>
       </c>
       <c r="D60" s="7">
-        <v>27.65</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,10 +1365,10 @@
         <v>13</v>
       </c>
       <c r="C61" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="D61" s="7">
         <v>27.9</v>
-      </c>
-      <c r="D61" s="7">
-        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,10 +1379,10 @@
         <v>14</v>
       </c>
       <c r="C62" s="7">
-        <v>28</v>
+        <v>27.9</v>
       </c>
       <c r="D62" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
         <v>22</v>
       </c>
       <c r="C63" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>10</v>
@@ -1438,7 +1438,7 @@
         <v>26.6</v>
       </c>
       <c r="D66" s="7">
-        <v>27.1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>27.25</v>
       </c>
       <c r="D67" s="7">
-        <v>27.65</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1463,10 +1463,10 @@
         <v>13</v>
       </c>
       <c r="C68" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="D68" s="7">
         <v>27.9</v>
-      </c>
-      <c r="D68" s="7">
-        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,10 +1477,10 @@
         <v>14</v>
       </c>
       <c r="C69" s="7">
-        <v>28</v>
+        <v>27.9</v>
       </c>
       <c r="D69" s="7">
-        <v>28.1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,7 +1491,7 @@
         <v>22</v>
       </c>
       <c r="C70" s="8">
-        <v>28.1</v>
+        <v>28</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>10</v>
@@ -1536,7 +1536,7 @@
         <v>27.25</v>
       </c>
       <c r="D73" s="7">
-        <v>27.55</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,10 +1547,10 @@
         <v>13</v>
       </c>
       <c r="C74" s="7">
-        <v>27.9</v>
+        <v>27.85</v>
       </c>
       <c r="D74" s="7">
-        <v>28</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1561,10 +1561,10 @@
         <v>14</v>
       </c>
       <c r="C75" s="7">
-        <v>28</v>
+        <v>27.95</v>
       </c>
       <c r="D75" s="7">
-        <v>28.1</v>
+        <v>28.05</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
         <v>22</v>
       </c>
       <c r="C76" s="7">
-        <v>28.1</v>
+        <v>28.05</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>10</v>

</xml_diff>